<commit_message>
Update assumption for MCH ideal case
Update hydrogen cost for MCH ideal case in input spreadsheet.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_test.xlsx
+++ b/systems2atoms/systems/inputs/input_params_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="967" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCAA3B45-0B25-43D9-A04B-D2AE1350F7D4}"/>
+  <xr:revisionPtr revIDLastSave="977" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3B9F197-F8A5-4847-9496-B19D5262C25E}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -975,6 +975,36 @@
           </rPr>
           <t xml:space="preserve">
 Based on assumption for MCH/toluene hydrogenation and dehydrogenation catalysts from Breunig et al., 2024, Nat Comm: https://www.nature.com/articles/s41467-024-53189-2.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{B1DC4FBD-5F3D-46E9-BBB8-7F7AD3A63FF4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hydrogen source for electrochemical production of MCH is 1 M sulfuric acid solution.
+Assumptions: 
+1. H2SO4 : H2 = 1 : 1. 
+2. Price of H2SO4 at 98% purity = $120/metric ton.
+3. Cost of water is negligible.
+https://www.chemanalyst.com/Pricing-data/sulphuric-acid-70
+https://businessanalytiq.com/procurementanalytics/index/sulfuric-acid-price-index/</t>
         </r>
       </text>
     </comment>
@@ -2313,10 +2343,10 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3239,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.31</v>
+        <v>6</v>
       </c>
       <c r="O6">
         <v>0</v>

</xml_diff>

<commit_message>
Update notes in input_prarams_test.xlsx
Make minor text change in notes in input spreadsheet.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_test.xlsx
+++ b/systems2atoms/systems/inputs/input_params_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="977" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3B9F197-F8A5-4847-9496-B19D5262C25E}"/>
+  <xr:revisionPtr revIDLastSave="985" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E466E05-7AA3-4FA5-8527-930970D1609A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,17 +229,22 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
+Accepted values are "thermo", "electro", or "purchase".
+Currently "thermo" LOHC production calculations are incomplete.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{CE96F9E7-E862-4E63-9E2A-7C2E1947B8B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Accepted values are "thermo", "electro", or "purchase".
-</t>
+          <t>Yuan, Mengyao:</t>
         </r>
         <r>
           <rPr>
@@ -249,122 +254,33 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
+Currently not used.
+Intended for "thermo" LOHC production calculations, which are currently incomplete.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{138103C3-8219-4014-8B1C-89126F5B990C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Currently "thermo" formic acid production calculations are incomplete.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{CE96F9E7-E862-4E63-9E2A-7C2E1947B8B3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
+          <t>Yuan, Mengyao:</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Yuan, Mengyao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Currently not used.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Intended for "thermo" formic acid production calculations, which are currently incomplete.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{138103C3-8219-4014-8B1C-89126F5B990C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yuan, Mengyao:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Placeholder.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+          <t xml:space="preserve">
+Placeholder.
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -389,7 +305,7 @@
           </rPr>
           <t xml:space="preserve">
 Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -414,7 +330,7 @@
           </rPr>
           <t xml:space="preserve">
 Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -439,7 +355,7 @@
           </rPr>
           <t xml:space="preserve">
 Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -464,7 +380,7 @@
           </rPr>
           <t xml:space="preserve">
 Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -489,7 +405,7 @@
           </rPr>
           <t xml:space="preserve">
 Placeholder.
-Used for "thermo" formic acid production calculations, which are currently incomplete.</t>
+Used for "thermo" LOHC production calculations, which are currently incomplete.</t>
         </r>
       </text>
     </comment>
@@ -2343,10 +2259,10 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3639,6 +3555,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
@@ -3647,15 +3572,6 @@
     <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3679,6 +3595,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3694,12 +3618,4 @@
     <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update hydrogen purchase cost assumption
Change hydrogen purchase cost ($/kg) to 0 for MCH ideal case. Rationale: water is the hydrogen source for toluene electro-hydrogenation (not H2SO4), and the estimated $/kg H2 is small based on California water rates.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_test.xlsx
+++ b/systems2atoms/systems/inputs/input_params_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="985" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E466E05-7AA3-4FA5-8527-930970D1609A}"/>
+  <xr:revisionPtr revIDLastSave="993" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68E9D3D9-5B94-4752-8FB1-692EFE7A0DE3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -894,7 +894,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{B1DC4FBD-5F3D-46E9-BBB8-7F7AD3A63FF4}">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{5E8EDE31-EEDA-4EF7-ABB4-9706B5D69D9C}">
       <text>
         <r>
           <rPr>
@@ -914,13 +914,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Hydrogen source for electrochemical production of MCH is 1 M sulfuric acid solution.
-Assumptions: 
-1. H2SO4 : H2 = 1 : 1. 
-2. Price of H2SO4 at 98% purity = $120/metric ton.
-3. Cost of water is negligible.
-https://www.chemanalyst.com/Pricing-data/sulphuric-acid-70
-https://businessanalytiq.com/procurementanalytics/index/sulfuric-acid-price-index/</t>
+Hydrogen source is water. Assume negligible on a $/kg H2 basis (a few cents per kg H2, estimated using California water rates).</t>
         </r>
       </text>
     </comment>
@@ -1959,6 +1953,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2259,10 +2257,10 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -3555,15 +3553,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="72d00a49-d4df-4ae2-8448-0e7c38748169">
@@ -3572,6 +3561,15 @@
     <TaxCatchAll xmlns="cdbd341c-9425-4527-8200-dbc5093c0c26" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3595,14 +3593,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA3A8468-9818-4804-84E1-135F70628E6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3618,4 +3608,12 @@
     <ds:schemaRef ds:uri="72d00a49-d4df-4ae2-8448-0e7c38748169"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB52D826-44CA-4104-AA1D-CE7759CCAD0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>